<commit_message>
`Tested Octree for radius seaches.
Octrees were much faster to construct, and had much faster query times
for radius neighborhood searches. Also able to control their properties
(i.e. maxiumum leaf population, leaf resolution) considering the scale of operations.

Going to change some implementations to octrees catered for feature
scales, instead of using kdtrees.
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PMD_Working\Dev\Projects\pcl_1.12_all_install\GeoDetection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357E04B8-F162-4440-944E-A73F6BB4BB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F71364-7FF4-4F73-9EA8-77345E1E6568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C49BB1A5-9B1C-4197-9CE5-B3BD3061C6DE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>Scale (m)</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Radius Search Demeaned (KdTree, OMP)</t>
+  </si>
+  <si>
+    <t>Radius Search Demeaned (Octree, OMP)</t>
   </si>
 </sst>
 </file>
@@ -130,10 +133,10 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A2AA5F-8CB2-4738-8100-FE6486C01FEA}">
-  <dimension ref="A2:H8"/>
+  <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,24 +470,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -519,7 +522,7 @@
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>79057628</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -528,14 +531,14 @@
       <c r="E5" s="2">
         <v>1</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>1736109.2005</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <f>F5/1000</f>
         <v>1736.1092005</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <f>G5/60</f>
         <v>28.935153341666666</v>
       </c>
@@ -547,7 +550,7 @@
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>79057628</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -556,14 +559,14 @@
       <c r="E6" s="2">
         <v>1</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>2948444.6855000001</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <f>F6/1000</f>
         <v>2948.4446855000001</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <f>G6/60</f>
         <v>49.140744758333334</v>
       </c>
@@ -575,23 +578,23 @@
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>79057628</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>0.5</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>444775.21350000001</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <f>F7/1000</f>
         <v>444.77521350000001</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <f>G7/60</f>
         <v>7.4129202249999997</v>
       </c>
@@ -603,25 +606,137 @@
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>79057628</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>0.25</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>203774.39929999999</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <f>F8/1000</f>
         <v>203.7743993</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <f>G8/60</f>
         <v>3.3962399883333334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>44460</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4">
+        <v>79057628</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
+      <c r="F9" s="4">
+        <v>7540197.5159999998</v>
+      </c>
+      <c r="G9" s="4">
+        <f>F9/1000</f>
+        <v>7540.1975160000002</v>
+      </c>
+      <c r="H9" s="4">
+        <f>G9/60</f>
+        <v>125.6699586</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>44460</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4">
+        <v>79057628</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F10" s="4">
+        <v>74567.853900000002</v>
+      </c>
+      <c r="G10" s="4">
+        <f>F10/1000</f>
+        <v>74.567853900000003</v>
+      </c>
+      <c r="H10" s="4">
+        <f>G10/60</f>
+        <v>1.242797565</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>44460</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="4">
+        <v>79057628</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2</v>
+      </c>
+      <c r="F11" s="4">
+        <v>2438933.4923999999</v>
+      </c>
+      <c r="G11" s="4">
+        <f>F11/1000</f>
+        <v>2438.9334924</v>
+      </c>
+      <c r="H11" s="4">
+        <f>G11/60</f>
+        <v>40.648891540000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>44460</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="4">
+        <v>79057628</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4">
+        <v>617709.61659999995</v>
+      </c>
+      <c r="G12" s="4">
+        <f>F12/1000</f>
+        <v>617.7096166</v>
+      </c>
+      <c r="H12" s="4">
+        <f>G12/60</f>
+        <v>10.295160276666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>